<commit_message>
CARLA-5 initial DD and DPE for P1 and P2
</commit_message>
<xml_diff>
--- a/rmonize/data_dictionary/DD_CARLA_P1.xlsx
+++ b/rmonize/data_dictionary/DD_CARLA_P1.xlsx
@@ -352,7 +352,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D11"/>
+  <dimension ref="A1:D110"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -391,7 +391,7 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>ID of the participant</t>
+          <t>ID</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -466,12 +466,12 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>occup_edu</t>
+          <t>occup_edu_h</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>First professional qualification</t>
+          <t>Highest professional qualification</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
@@ -486,17 +486,17 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>occup_edu_2</t>
+          <t>met_we</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Second professional qualification</t>
+          <t>MET per week</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>integer</t>
+          <t>decimal</t>
         </is>
       </c>
     </row>
@@ -506,17 +506,17 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>met_we</t>
+          <t>smoker</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>MET per week</t>
+          <t>smoker</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>decimal</t>
+          <t>integer</t>
         </is>
       </c>
     </row>
@@ -526,17 +526,17 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>smoker</t>
+          <t>bmi</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>smoker</t>
+          <t>bmi</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>integer</t>
+          <t>decimal</t>
         </is>
       </c>
     </row>
@@ -546,12 +546,12 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>bmi</t>
+          <t>gj</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>bmi</t>
+          <t>Gesamtenergie [kJ/Tag]</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
@@ -566,15 +566,1995 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>gj</t>
+          <t>POTATOES_TUB_01</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>total energy intake at baseline</t>
+          <t>Intake of starchy roots or tubers [g/d]</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
+        <is>
+          <t>decimal</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>POTATOES_0101</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>Potato intake [g/d]</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>decimal</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>VEGETABLES_02</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>Vegetable intake [g/d]</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>decimal</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>LEAFYVEG_0201</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>Leafy vegetable intake [g/d]</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>decimal</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>FRUITINGVEG_0202</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>Fruiting vegetable intake [g/d]</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>decimal</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>ROOTVEG_0203</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>Root and tuber vegetable intake [g/d]</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>decimal</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>CABBAGE_0204</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>Head cabbages and similar intake [g/d]</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>decimal</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>MUSHROOMS_0205</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>Mushroom intake [g/d]</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>decimal</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>GRAINPODVEG_0206</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>Intake of legumes with pod [g/d]</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>decimal</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20">
+        <v>19</v>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>ONION_GARLIC_0207</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>Bulb vegetables (onions, garlic) intake [g/d]</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>decimal</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21">
+        <v>20</v>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>STALKVEG_0208</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>Intake of stems/stalks eaten as vegetables [g/d]</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>decimal</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22">
+        <v>21</v>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>MIXEDVEG_0209</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>Intake of mixed vegetable salad or mixed green salad [g/d]</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>decimal</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23">
+        <v>22</v>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>LEGUMES_TOT_03</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>Total legumes intake [g/d]</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>decimal</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24">
+        <v>23</v>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>LEGUMES_0301</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>Intake fresh seeds (without pod) from legumes (beans, peas etc.) [g/d]</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>decimal</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25">
+        <v>24</v>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>FRUITS_TOT_04</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>Total fruit intake [g/d]</t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>decimal</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26">
+        <v>25</v>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>FRUITS_0401</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>Intake of fresh fruits [g/d]</t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>decimal</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27">
+        <v>26</v>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>NUTS_SEEDS_0402</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>Intake of tree nuts and seeds [g/d]</t>
+        </is>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>decimal</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28">
+        <v>27</v>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>MIXEDFRUITS_0403</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>Intake of candied fruit/mixed fruit, canned, jarred mixed fruit and miscellaneous fruits [g/d]</t>
+        </is>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>decimal</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29">
+        <v>28</v>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>DAIRY_05</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>Intake of milk and dairy products and milk and milk products (dairy) [g/d]</t>
+        </is>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>decimal</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30">
+        <v>29</v>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>MILK_0501</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>Intake of (whole) cow and cattle milk [g/d]</t>
+        </is>
+      </c>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>decimal</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31">
+        <v>30</v>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>MILKBEV_0502</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>Intake of buttermilk, traditional buttermilk, flavoured milk, flavoured whey and milk-based drinks (as part-nature) [g/d]</t>
+        </is>
+      </c>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>decimal</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32">
+        <v>31</v>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>YOGURT_0503</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>Intake of fermented milk products [g/d]</t>
+        </is>
+      </c>
+      <c r="D32" t="inlineStr">
+        <is>
+          <t>decimal</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33">
+        <v>32</v>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>CURD_0504</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>Intake of cheese curd, quark and cottage [g/d]</t>
+        </is>
+      </c>
+      <c r="D33" t="inlineStr">
+        <is>
+          <t>decimal</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34">
+        <v>33</v>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>CHEESE_0505</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>Intake of cheese [g/d]</t>
+        </is>
+      </c>
+      <c r="D34" t="inlineStr">
+        <is>
+          <t>decimal</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35">
+        <v>34</v>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>DAIRYDESSERT_0506</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>Intake of dairy dessert and similar starchy pudding [g/d]</t>
+        </is>
+      </c>
+      <c r="D35" t="inlineStr">
+        <is>
+          <t>decimal</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36">
+        <v>35</v>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>CREAM_PROD_0507</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>Intake of cream and cream products [g/d]</t>
+        </is>
+      </c>
+      <c r="D36" t="inlineStr">
+        <is>
+          <t>decimal</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37">
+        <v>36</v>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>DAIRYCREAM_050701</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>Cream intake (as part-nature) [g/d]</t>
+        </is>
+      </c>
+      <c r="D37" t="inlineStr">
+        <is>
+          <t>decimal</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38">
+        <v>37</v>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>MILK_FOR_COFFEE_0508</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>Intake of condensed milk (sometimes with added sugars) and milk and dairy powders and concentrates [g/d]</t>
+        </is>
+      </c>
+      <c r="D38" t="inlineStr">
+        <is>
+          <t>decimal</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39">
+        <v>38</v>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>CEREAL_PROD_06</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>Intake of cereals and cereal primary derivatives, cereal grains (and cereal-like grains) [g/d]</t>
+        </is>
+      </c>
+      <c r="D39" t="inlineStr">
+        <is>
+          <t>decimal</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40">
+        <v>39</v>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>FLOUR_FLAKES_0601</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>Intake of flours and other milled products and starches [g/d]</t>
+        </is>
+      </c>
+      <c r="D40" t="inlineStr">
+        <is>
+          <t>decimal</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41">
+        <v>40</v>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>PASTA_RICE_0602</t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>Intake of pastas and rice [g/d]</t>
+        </is>
+      </c>
+      <c r="D41" t="inlineStr">
+        <is>
+          <t>decimal</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42">
+        <v>41</v>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>BREAD_PROD_0603</t>
+        </is>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>Intake of bread and bread products [g/d]</t>
+        </is>
+      </c>
+      <c r="D42" t="inlineStr">
+        <is>
+          <t>decimal</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43">
+        <v>42</v>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>BREAD_060301</t>
+        </is>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>Intake of bread [g/d]</t>
+        </is>
+      </c>
+      <c r="D43" t="inlineStr">
+        <is>
+          <t>decimal</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44">
+        <v>43</v>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>CRISPBREAD_060302</t>
+        </is>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>Intake of crisp bread and rusk [g/d]</t>
+        </is>
+      </c>
+      <c r="D44" t="inlineStr">
+        <is>
+          <t>decimal</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45">
+        <v>44</v>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>BREAKF_CEREALS_0604</t>
+        </is>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>Intake of breakfast cereals [g/d]</t>
+        </is>
+      </c>
+      <c r="D45" t="inlineStr">
+        <is>
+          <t>decimal</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46">
+        <v>45</v>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>SALT_BISCUIT_0605</t>
+        </is>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>Intake of crackers and breadsticks [g/d]</t>
+        </is>
+      </c>
+      <c r="D46" t="inlineStr">
+        <is>
+          <t>decimal</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47">
+        <v>46</v>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>DOUGH_PASTRY_0606</t>
+        </is>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>Intake of fine bakery products [g/d]</t>
+        </is>
+      </c>
+      <c r="D47" t="inlineStr">
+        <is>
+          <t>decimal</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48">
+        <v>47</v>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>MEAT_PROD_07</t>
+        </is>
+      </c>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>Intake of meat and meat products [g/d]</t>
+        </is>
+      </c>
+      <c r="D48" t="inlineStr">
+        <is>
+          <t>decimal</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49">
+        <v>48</v>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>RED_MEAT_0701</t>
+        </is>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>Intake of red meat (mammals meat) [g/d]</t>
+        </is>
+      </c>
+      <c r="D49" t="inlineStr">
+        <is>
+          <t>decimal</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50">
+        <v>49</v>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>BEEF_070101</t>
+        </is>
+      </c>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>Intake of cow, ox or bull fresh meat [g/d]</t>
+        </is>
+      </c>
+      <c r="D50" t="inlineStr">
+        <is>
+          <t>decimal</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51">
+        <v>50</v>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>VEAL_070102</t>
+        </is>
+      </c>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>Intake of calf fresh meat [g/d]</t>
+        </is>
+      </c>
+      <c r="D51" t="inlineStr">
+        <is>
+          <t>decimal</t>
+        </is>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52">
+        <v>51</v>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>PORK_070103</t>
+        </is>
+      </c>
+      <c r="C52" t="inlineStr">
+        <is>
+          <t>Intake of pig fresh meat [g/d]</t>
+        </is>
+      </c>
+      <c r="D52" t="inlineStr">
+        <is>
+          <t>decimal</t>
+        </is>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53">
+        <v>52</v>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>MUTTON_LAMB_070104</t>
+        </is>
+      </c>
+      <c r="C53" t="inlineStr">
+        <is>
+          <t>Intake of lamb and sheep meat [g/d]</t>
+        </is>
+      </c>
+      <c r="D53" t="inlineStr">
+        <is>
+          <t>decimal</t>
+        </is>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54">
+        <v>53</v>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>POULTRY_0702</t>
+        </is>
+      </c>
+      <c r="C54" t="inlineStr">
+        <is>
+          <t>Intake of poultry meat [g/d]</t>
+        </is>
+      </c>
+      <c r="D54" t="inlineStr">
+        <is>
+          <t>decimal</t>
+        </is>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55">
+        <v>54</v>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>OTHERPOULTRY_070200</t>
+        </is>
+      </c>
+      <c r="C55" t="inlineStr">
+        <is>
+          <t>Intake of other poultry meat [g/d]</t>
+        </is>
+      </c>
+      <c r="D55" t="inlineStr">
+        <is>
+          <t>decimal</t>
+        </is>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56">
+        <v>55</v>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>CHICKEN_070201</t>
+        </is>
+      </c>
+      <c r="C56" t="inlineStr">
+        <is>
+          <t>Intake of chicken meat [g/d]</t>
+        </is>
+      </c>
+      <c r="D56" t="inlineStr">
+        <is>
+          <t>decimal</t>
+        </is>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57">
+        <v>56</v>
+      </c>
+      <c r="B57" t="inlineStr">
+        <is>
+          <t>RABBIT_070205</t>
+        </is>
+      </c>
+      <c r="C57" t="inlineStr">
+        <is>
+          <t>Intake of rabbit meat [g/d]</t>
+        </is>
+      </c>
+      <c r="D57" t="inlineStr">
+        <is>
+          <t>decimal</t>
+        </is>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58">
+        <v>57</v>
+      </c>
+      <c r="B58" t="inlineStr">
+        <is>
+          <t>PROCMEAT_0704</t>
+        </is>
+      </c>
+      <c r="C58" t="inlineStr">
+        <is>
+          <t>Intake of processed or preserved meat [g/d]</t>
+        </is>
+      </c>
+      <c r="D58" t="inlineStr">
+        <is>
+          <t>decimal</t>
+        </is>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59">
+        <v>58</v>
+      </c>
+      <c r="B59" t="inlineStr">
+        <is>
+          <t>OFFALS_0705</t>
+        </is>
+      </c>
+      <c r="C59" t="inlineStr">
+        <is>
+          <t>Intake of animal offal and other slaughtering [g/d]</t>
+        </is>
+      </c>
+      <c r="D59" t="inlineStr">
+        <is>
+          <t>decimal</t>
+        </is>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60">
+        <v>59</v>
+      </c>
+      <c r="B60" t="inlineStr">
+        <is>
+          <t>FISH_SHELLFISH_08</t>
+        </is>
+      </c>
+      <c r="C60" t="inlineStr">
+        <is>
+          <t>Intake of fish and seafood and products thereof [g/d]</t>
+        </is>
+      </c>
+      <c r="D60" t="inlineStr">
+        <is>
+          <t>decimal</t>
+        </is>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61">
+        <v>60</v>
+      </c>
+      <c r="B61" t="inlineStr">
+        <is>
+          <t>FISH_0801</t>
+        </is>
+      </c>
+      <c r="C61" t="inlineStr">
+        <is>
+          <t>Intake of fish (meat) [g/d]</t>
+        </is>
+      </c>
+      <c r="D61" t="inlineStr">
+        <is>
+          <t>decimal</t>
+        </is>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62">
+        <v>61</v>
+      </c>
+      <c r="B62" t="inlineStr">
+        <is>
+          <t>FISH_PROD_0803</t>
+        </is>
+      </c>
+      <c r="C62" t="inlineStr">
+        <is>
+          <t>Intake of processed fish [g/d]</t>
+        </is>
+      </c>
+      <c r="D62" t="inlineStr">
+        <is>
+          <t>decimal</t>
+        </is>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63">
+        <v>62</v>
+      </c>
+      <c r="B63" t="inlineStr">
+        <is>
+          <t>EGG_PROD_09</t>
+        </is>
+      </c>
+      <c r="C63" t="inlineStr">
+        <is>
+          <t>Intake of eggs and egg products [g/d]</t>
+        </is>
+      </c>
+      <c r="D63" t="inlineStr">
+        <is>
+          <t>decimal</t>
+        </is>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64">
+        <v>63</v>
+      </c>
+      <c r="B64" t="inlineStr">
+        <is>
+          <t>EGGS_0901</t>
+        </is>
+      </c>
+      <c r="C64" t="inlineStr">
+        <is>
+          <t>Intake of eggs [g/d]</t>
+        </is>
+      </c>
+      <c r="D64" t="inlineStr">
+        <is>
+          <t>decimal</t>
+        </is>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65">
+        <v>64</v>
+      </c>
+      <c r="B65" t="inlineStr">
+        <is>
+          <t>FAT_10</t>
+        </is>
+      </c>
+      <c r="C65" t="inlineStr">
+        <is>
+          <t>Intake of animal and vegetable fats and oils [g/d]</t>
+        </is>
+      </c>
+      <c r="D65" t="inlineStr">
+        <is>
+          <t>decimal</t>
+        </is>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66">
+        <v>65</v>
+      </c>
+      <c r="B66" t="inlineStr">
+        <is>
+          <t>VEGOILS_1001</t>
+        </is>
+      </c>
+      <c r="C66" t="inlineStr">
+        <is>
+          <t>Intake of vegetable fats and oils [g/d]</t>
+        </is>
+      </c>
+      <c r="D66" t="inlineStr">
+        <is>
+          <t>decimal</t>
+        </is>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67">
+        <v>66</v>
+      </c>
+      <c r="B67" t="inlineStr">
+        <is>
+          <t>BUTTER_1002</t>
+        </is>
+      </c>
+      <c r="C67" t="inlineStr">
+        <is>
+          <t>Intake of butter [g/d]</t>
+        </is>
+      </c>
+      <c r="D67" t="inlineStr">
+        <is>
+          <t>decimal</t>
+        </is>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68">
+        <v>67</v>
+      </c>
+      <c r="B68" t="inlineStr">
+        <is>
+          <t>MARGARINE_1003</t>
+        </is>
+      </c>
+      <c r="C68" t="inlineStr">
+        <is>
+          <t>Intake of margarines and similar [g/d]</t>
+        </is>
+      </c>
+      <c r="D68" t="inlineStr">
+        <is>
+          <t>decimal</t>
+        </is>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69">
+        <v>68</v>
+      </c>
+      <c r="B69" t="inlineStr">
+        <is>
+          <t>FRYFAT_1004</t>
+        </is>
+      </c>
+      <c r="C69" t="inlineStr">
+        <is>
+          <t>Intake of blended frying oil/fats [g/d]</t>
+        </is>
+      </c>
+      <c r="D69" t="inlineStr">
+        <is>
+          <t>decimal</t>
+        </is>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70">
+        <v>69</v>
+      </c>
+      <c r="B70" t="inlineStr">
+        <is>
+          <t>OTHER_ANIMALFAT_1006</t>
+        </is>
+      </c>
+      <c r="C70" t="inlineStr">
+        <is>
+          <t>Intake of animal fats (processed fat from animal tissue) [g/d]</t>
+        </is>
+      </c>
+      <c r="D70" t="inlineStr">
+        <is>
+          <t>decimal</t>
+        </is>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71">
+        <v>70</v>
+      </c>
+      <c r="B71" t="inlineStr">
+        <is>
+          <t>SUGAR_CONFECT_11</t>
+        </is>
+      </c>
+      <c r="C71" t="inlineStr">
+        <is>
+          <t>Intake of sugar and similar, confectionery and water-based sweet desserts [g/d]</t>
+        </is>
+      </c>
+      <c r="D71" t="inlineStr">
+        <is>
+          <t>decimal</t>
+        </is>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72">
+        <v>71</v>
+      </c>
+      <c r="B72" t="inlineStr">
+        <is>
+          <t>HONEY_JAM_1101</t>
+        </is>
+      </c>
+      <c r="C72" t="inlineStr">
+        <is>
+          <t>Intake of sugars, syrups, honey and table-top sweeteners [g/d]</t>
+        </is>
+      </c>
+      <c r="D72" t="inlineStr">
+        <is>
+          <t>decimal</t>
+        </is>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73">
+        <v>72</v>
+      </c>
+      <c r="B73" t="inlineStr">
+        <is>
+          <t>CHOCOLATE_1102</t>
+        </is>
+      </c>
+      <c r="C73" t="inlineStr">
+        <is>
+          <t>Intake of chocolate, chocolate products and chocolate coated confectionary [g/d]</t>
+        </is>
+      </c>
+      <c r="D73" t="inlineStr">
+        <is>
+          <t>decimal</t>
+        </is>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74">
+        <v>73</v>
+      </c>
+      <c r="B74" t="inlineStr">
+        <is>
+          <t>NONCHOC_SWEETS_1103</t>
+        </is>
+      </c>
+      <c r="C74" t="inlineStr">
+        <is>
+          <t>Intake of sweet bars and other formed sweet masses, candies (soft and hard) and other confectionery including breath refreshening microsweets [g/d]</t>
+        </is>
+      </c>
+      <c r="D74" t="inlineStr">
+        <is>
+          <t>decimal</t>
+        </is>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75">
+        <v>74</v>
+      </c>
+      <c r="B75" t="inlineStr">
+        <is>
+          <t>ICECREAM_1105</t>
+        </is>
+      </c>
+      <c r="C75" t="inlineStr">
+        <is>
+          <t>Intake of spoonable desserts and ice creams [g/d]</t>
+        </is>
+      </c>
+      <c r="D75" t="inlineStr">
+        <is>
+          <t>decimal</t>
+        </is>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76">
+        <v>75</v>
+      </c>
+      <c r="B76" t="inlineStr">
+        <is>
+          <t>ICECREAM_MILK_110501</t>
+        </is>
+      </c>
+      <c r="C76" t="inlineStr">
+        <is>
+          <t>Intake of milk-based ice cream [g/d]</t>
+        </is>
+      </c>
+      <c r="D76" t="inlineStr">
+        <is>
+          <t>decimal</t>
+        </is>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77">
+        <v>76</v>
+      </c>
+      <c r="B77" t="inlineStr">
+        <is>
+          <t>CAKES_12</t>
+        </is>
+      </c>
+      <c r="C77" t="inlineStr">
+        <is>
+          <t>Intake of cakes and fine bakery products [g/d]</t>
+        </is>
+      </c>
+      <c r="D77" t="inlineStr">
+        <is>
+          <t>decimal</t>
+        </is>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78">
+        <v>77</v>
+      </c>
+      <c r="B78" t="inlineStr">
+        <is>
+          <t>VARPASTRY_1201</t>
+        </is>
+      </c>
+      <c r="C78" t="inlineStr">
+        <is>
+          <t>Intake of various pastry [g/d]</t>
+        </is>
+      </c>
+      <c r="D78" t="inlineStr">
+        <is>
+          <t>decimal</t>
+        </is>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79">
+        <v>78</v>
+      </c>
+      <c r="B79" t="inlineStr">
+        <is>
+          <t>DRYCAKE_1202</t>
+        </is>
+      </c>
+      <c r="C79" t="inlineStr">
+        <is>
+          <t>Intake of sponge biscuits and plain cakes [g/d]</t>
+        </is>
+      </c>
+      <c r="D79" t="inlineStr">
+        <is>
+          <t>decimal</t>
+        </is>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80">
+        <v>79</v>
+      </c>
+      <c r="B80" t="inlineStr">
+        <is>
+          <t>NONALC_BEV_13</t>
+        </is>
+      </c>
+      <c r="C80" t="inlineStr">
+        <is>
+          <t>Intake of non-alcoholic beverages [g/d]</t>
+        </is>
+      </c>
+      <c r="D80" t="inlineStr">
+        <is>
+          <t>decimal</t>
+        </is>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81">
+        <v>80</v>
+      </c>
+      <c r="B81" t="inlineStr">
+        <is>
+          <t>FRUITVEG_JUICE_1301</t>
+        </is>
+      </c>
+      <c r="C81" t="inlineStr">
+        <is>
+          <t>Intake of fruit and vegetable juices [g/d]</t>
+        </is>
+      </c>
+      <c r="D81" t="inlineStr">
+        <is>
+          <t>decimal</t>
+        </is>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82">
+        <v>81</v>
+      </c>
+      <c r="B82" t="inlineStr">
+        <is>
+          <t>SOFTDRINKS_1302</t>
+        </is>
+      </c>
+      <c r="C82" t="inlineStr">
+        <is>
+          <t>Intake of soft drinks [g/d]</t>
+        </is>
+      </c>
+      <c r="D82" t="inlineStr">
+        <is>
+          <t>decimal</t>
+        </is>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83">
+        <v>82</v>
+      </c>
+      <c r="B83" t="inlineStr">
+        <is>
+          <t>HOTDRINKS_1303</t>
+        </is>
+      </c>
+      <c r="C83" t="inlineStr">
+        <is>
+          <t>Intake of hot drinks and similar (coffee, cocoa, tea and herbal infusions) [g/d]</t>
+        </is>
+      </c>
+      <c r="D83" t="inlineStr">
+        <is>
+          <t>decimal</t>
+        </is>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84">
+        <v>83</v>
+      </c>
+      <c r="B84" t="inlineStr">
+        <is>
+          <t>COFFEE_130301</t>
+        </is>
+      </c>
+      <c r="C84" t="inlineStr">
+        <is>
+          <t>Coffee intake [g/d]</t>
+        </is>
+      </c>
+      <c r="D84" t="inlineStr">
+        <is>
+          <t>decimal</t>
+        </is>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85">
+        <v>84</v>
+      </c>
+      <c r="B85" t="inlineStr">
+        <is>
+          <t>TEA_130302</t>
+        </is>
+      </c>
+      <c r="C85" t="inlineStr">
+        <is>
+          <t>Tea intake [g/d]</t>
+        </is>
+      </c>
+      <c r="D85" t="inlineStr">
+        <is>
+          <t>decimal</t>
+        </is>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86">
+        <v>85</v>
+      </c>
+      <c r="B86" t="inlineStr">
+        <is>
+          <t>HERBALTEA_130303</t>
+        </is>
+      </c>
+      <c r="C86" t="inlineStr">
+        <is>
+          <t>Intake of herbal and other non-tea infusions [g/d]</t>
+        </is>
+      </c>
+      <c r="D86" t="inlineStr">
+        <is>
+          <t>decimal</t>
+        </is>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87">
+        <v>86</v>
+      </c>
+      <c r="B87" t="inlineStr">
+        <is>
+          <t>COFFEE_IMITATE_130304</t>
+        </is>
+      </c>
+      <c r="C87" t="inlineStr">
+        <is>
+          <t>Intake of chicory coffee infusion and coffee imitate beverages [g/d]</t>
+        </is>
+      </c>
+      <c r="D87" t="inlineStr">
+        <is>
+          <t>decimal</t>
+        </is>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88">
+        <v>87</v>
+      </c>
+      <c r="B88" t="inlineStr">
+        <is>
+          <t>WATER_1304</t>
+        </is>
+      </c>
+      <c r="C88" t="inlineStr">
+        <is>
+          <t>Intake of water and water-based beverages [g/d]</t>
+        </is>
+      </c>
+      <c r="D88" t="inlineStr">
+        <is>
+          <t>decimal</t>
+        </is>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89">
+        <v>88</v>
+      </c>
+      <c r="B89" t="inlineStr">
+        <is>
+          <t>ALC_BEV_14</t>
+        </is>
+      </c>
+      <c r="C89" t="inlineStr">
+        <is>
+          <t>Alcoholic beverage intake [g/d]</t>
+        </is>
+      </c>
+      <c r="D89" t="inlineStr">
+        <is>
+          <t>decimal</t>
+        </is>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90">
+        <v>89</v>
+      </c>
+      <c r="B90" t="inlineStr">
+        <is>
+          <t>WINE_1401</t>
+        </is>
+      </c>
+      <c r="C90" t="inlineStr">
+        <is>
+          <t>Intake of wine and wine-like drinks [g/d]</t>
+        </is>
+      </c>
+      <c r="D90" t="inlineStr">
+        <is>
+          <t>decimal</t>
+        </is>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91">
+        <v>90</v>
+      </c>
+      <c r="B91" t="inlineStr">
+        <is>
+          <t>FORTWINE_1402</t>
+        </is>
+      </c>
+      <c r="C91" t="inlineStr">
+        <is>
+          <t>Intake of fortified/liqueur wine [g/d]</t>
+        </is>
+      </c>
+      <c r="D91" t="inlineStr">
+        <is>
+          <t>decimal</t>
+        </is>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92">
+        <v>91</v>
+      </c>
+      <c r="B92" t="inlineStr">
+        <is>
+          <t>BEER_1403</t>
+        </is>
+      </c>
+      <c r="C92" t="inlineStr">
+        <is>
+          <t>Intake of beer and beer-like beverage [g/d]</t>
+        </is>
+      </c>
+      <c r="D92" t="inlineStr">
+        <is>
+          <t>decimal</t>
+        </is>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93">
+        <v>92</v>
+      </c>
+      <c r="B93" t="inlineStr">
+        <is>
+          <t>SPIRITS_1404</t>
+        </is>
+      </c>
+      <c r="C93" t="inlineStr">
+        <is>
+          <t>Intake of unsweetened spirits [g/d]</t>
+        </is>
+      </c>
+      <c r="D93" t="inlineStr">
+        <is>
+          <t>decimal</t>
+        </is>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94">
+        <v>93</v>
+      </c>
+      <c r="B94" t="inlineStr">
+        <is>
+          <t>HERBLIQUEUR_1405</t>
+        </is>
+      </c>
+      <c r="C94" t="inlineStr">
+        <is>
+          <t>Intake of herb liqueur [g/d]</t>
+        </is>
+      </c>
+      <c r="D94" t="inlineStr">
+        <is>
+          <t>decimal</t>
+        </is>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95">
+        <v>94</v>
+      </c>
+      <c r="B95" t="inlineStr">
+        <is>
+          <t>LIQUEURS_1406</t>
+        </is>
+      </c>
+      <c r="C95" t="inlineStr">
+        <is>
+          <t>Intake of liqueurs [g/d]</t>
+        </is>
+      </c>
+      <c r="D95" t="inlineStr">
+        <is>
+          <t>decimal</t>
+        </is>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96">
+        <v>95</v>
+      </c>
+      <c r="B96" t="inlineStr">
+        <is>
+          <t>CONDIMENT_SAUCES_15</t>
+        </is>
+      </c>
+      <c r="C96" t="inlineStr">
+        <is>
+          <t>Intake of seasoning, sauces and condiments [g/d]</t>
+        </is>
+      </c>
+      <c r="D96" t="inlineStr">
+        <is>
+          <t>decimal</t>
+        </is>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97">
+        <v>96</v>
+      </c>
+      <c r="B97" t="inlineStr">
+        <is>
+          <t>SAUCES_1501</t>
+        </is>
+      </c>
+      <c r="C97" t="inlineStr">
+        <is>
+          <t>Intake of savoury sauces [g/d]</t>
+        </is>
+      </c>
+      <c r="D97" t="inlineStr">
+        <is>
+          <t>decimal</t>
+        </is>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98">
+        <v>97</v>
+      </c>
+      <c r="B98" t="inlineStr">
+        <is>
+          <t>TOMATOSAUCE_150101</t>
+        </is>
+      </c>
+      <c r="C98" t="inlineStr">
+        <is>
+          <t>Intake of tomato-containing cooked sauces [g/d]</t>
+        </is>
+      </c>
+      <c r="D98" t="inlineStr">
+        <is>
+          <t>decimal</t>
+        </is>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99">
+        <v>98</v>
+      </c>
+      <c r="B99" t="inlineStr">
+        <is>
+          <t>DRESSINGS_150102</t>
+        </is>
+      </c>
+      <c r="C99" t="inlineStr">
+        <is>
+          <t>Dressing intake [g/d]</t>
+        </is>
+      </c>
+      <c r="D99" t="inlineStr">
+        <is>
+          <t>decimal</t>
+        </is>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100">
+        <v>99</v>
+      </c>
+      <c r="B100" t="inlineStr">
+        <is>
+          <t>MAYONNAISE_150103</t>
+        </is>
+      </c>
+      <c r="C100" t="inlineStr">
+        <is>
+          <t>Intake of mayonnaise [g/d]</t>
+        </is>
+      </c>
+      <c r="D100" t="inlineStr">
+        <is>
+          <t>decimal</t>
+        </is>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101">
+        <v>100</v>
+      </c>
+      <c r="B101" t="inlineStr">
+        <is>
+          <t>HERBS_SPICES_1503</t>
+        </is>
+      </c>
+      <c r="C101" t="inlineStr">
+        <is>
+          <t>Intakes of berbs, spices and similar [g/d]</t>
+        </is>
+      </c>
+      <c r="D101" t="inlineStr">
+        <is>
+          <t>decimal</t>
+        </is>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102">
+        <v>101</v>
+      </c>
+      <c r="B102" t="inlineStr">
+        <is>
+          <t>CONDIMENTS_1504</t>
+        </is>
+      </c>
+      <c r="C102" t="inlineStr">
+        <is>
+          <t>Condiments intake [g/d]</t>
+        </is>
+      </c>
+      <c r="D102" t="inlineStr">
+        <is>
+          <t>decimal</t>
+        </is>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103">
+        <v>102</v>
+      </c>
+      <c r="B103" t="inlineStr">
+        <is>
+          <t>SOUP_BOUILLON_16</t>
+        </is>
+      </c>
+      <c r="C103" t="inlineStr">
+        <is>
+          <t>Intake of soups and broths [g/d]</t>
+        </is>
+      </c>
+      <c r="D103" t="inlineStr">
+        <is>
+          <t>decimal</t>
+        </is>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104">
+        <v>103</v>
+      </c>
+      <c r="B104" t="inlineStr">
+        <is>
+          <t>SOUP_1601</t>
+        </is>
+      </c>
+      <c r="C104" t="inlineStr">
+        <is>
+          <t>Intake of soups [g/d]</t>
+        </is>
+      </c>
+      <c r="D104" t="inlineStr">
+        <is>
+          <t>decimal</t>
+        </is>
+      </c>
+    </row>
+    <row r="105">
+      <c r="A105">
+        <v>104</v>
+      </c>
+      <c r="B105" t="inlineStr">
+        <is>
+          <t>BOUILLON_1602</t>
+        </is>
+      </c>
+      <c r="C105" t="inlineStr">
+        <is>
+          <t>Intake of mixed vegetables soup, clear meat soup [g/d]</t>
+        </is>
+      </c>
+      <c r="D105" t="inlineStr">
+        <is>
+          <t>decimal</t>
+        </is>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106">
+        <v>105</v>
+      </c>
+      <c r="B106" t="inlineStr">
+        <is>
+          <t>MISCELLANEOUS_17</t>
+        </is>
+      </c>
+      <c r="C106" t="inlineStr">
+        <is>
+          <t>Intake of miscellaneous [g/d]</t>
+        </is>
+      </c>
+      <c r="D106" t="inlineStr">
+        <is>
+          <t>decimal</t>
+        </is>
+      </c>
+    </row>
+    <row r="107">
+      <c r="A107">
+        <v>106</v>
+      </c>
+      <c r="B107" t="inlineStr">
+        <is>
+          <t>VEG_DISHES_1700</t>
+        </is>
+      </c>
+      <c r="C107" t="inlineStr">
+        <is>
+          <t>Intake of vegetarian products and dishes [g/d]</t>
+        </is>
+      </c>
+      <c r="D107" t="inlineStr">
+        <is>
+          <t>decimal</t>
+        </is>
+      </c>
+    </row>
+    <row r="108">
+      <c r="A108">
+        <v>107</v>
+      </c>
+      <c r="B108" t="inlineStr">
+        <is>
+          <t>SOY_PROD_1701</t>
+        </is>
+      </c>
+      <c r="C108" t="inlineStr">
+        <is>
+          <t>Intake of soy products [g/d]</t>
+        </is>
+      </c>
+      <c r="D108" t="inlineStr">
+        <is>
+          <t>decimal</t>
+        </is>
+      </c>
+    </row>
+    <row r="109">
+      <c r="A109">
+        <v>108</v>
+      </c>
+      <c r="B109" t="inlineStr">
+        <is>
+          <t>DIET_PROD_1702</t>
+        </is>
+      </c>
+      <c r="C109" t="inlineStr">
+        <is>
+          <t>Intake of food for weight reduction [g/d]</t>
+        </is>
+      </c>
+      <c r="D109" t="inlineStr">
+        <is>
+          <t>decimal</t>
+        </is>
+      </c>
+    </row>
+    <row r="110">
+      <c r="A110">
+        <v>109</v>
+      </c>
+      <c r="B110" t="inlineStr">
+        <is>
+          <t>ART_SWEETENER_170201</t>
+        </is>
+      </c>
+      <c r="C110" t="inlineStr">
+        <is>
+          <t>Intake of artificial sweeteners (e.g., aspartam, saccharine) [g/d]</t>
+        </is>
+      </c>
+      <c r="D110" t="inlineStr">
         <is>
           <t>decimal</t>
         </is>
@@ -587,7 +2567,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C29"/>
+  <dimension ref="A1:C21"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -666,7 +2646,7 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>elementary School</t>
+          <t>Hauptschule</t>
         </is>
       </c>
     </row>
@@ -748,7 +2728,7 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>occup_edu</t>
+          <t>occup_edu_h</t>
         </is>
       </c>
       <c r="B11">
@@ -763,7 +2743,7 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>occup_edu</t>
+          <t>occup_edu_h</t>
         </is>
       </c>
       <c r="B12">
@@ -778,7 +2758,7 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>occup_edu</t>
+          <t>occup_edu_h</t>
         </is>
       </c>
       <c r="B13">
@@ -793,7 +2773,7 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>occup_edu</t>
+          <t>occup_edu_h</t>
         </is>
       </c>
       <c r="B14">
@@ -808,7 +2788,7 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>occup_edu</t>
+          <t>occup_edu_h</t>
         </is>
       </c>
       <c r="B15">
@@ -823,7 +2803,7 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>occup_edu</t>
+          <t>occup_edu_h</t>
         </is>
       </c>
       <c r="B16">
@@ -838,7 +2818,7 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>occup_edu</t>
+          <t>occup_edu_h</t>
         </is>
       </c>
       <c r="B17">
@@ -853,7 +2833,7 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>occup_edu</t>
+          <t>occup_edu_h</t>
         </is>
       </c>
       <c r="B18">
@@ -868,7 +2848,7 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>occup_edu_2</t>
+          <t>smoker</t>
         </is>
       </c>
       <c r="B19">
@@ -876,14 +2856,14 @@
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>no vocational education</t>
+          <t>Current Smoker</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>occup_edu_2</t>
+          <t>smoker</t>
         </is>
       </c>
       <c r="B20">
@@ -891,140 +2871,20 @@
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>training period</t>
+          <t>Ex Smoker</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>occup_edu_2</t>
+          <t>smoker</t>
         </is>
       </c>
       <c r="B21">
         <v>3</v>
       </c>
       <c r="C21" t="inlineStr">
-        <is>
-          <t>apprenticeship(Lehre)</t>
-        </is>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" t="inlineStr">
-        <is>
-          <t>occup_edu_2</t>
-        </is>
-      </c>
-      <c r="B22">
-        <v>4</v>
-      </c>
-      <c r="C22" t="inlineStr">
-        <is>
-          <t>vocational school(Berufsschule)</t>
-        </is>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" t="inlineStr">
-        <is>
-          <t>occup_edu_2</t>
-        </is>
-      </c>
-      <c r="B23">
-        <v>5</v>
-      </c>
-      <c r="C23" t="inlineStr">
-        <is>
-          <t>technical school(Fachschule)</t>
-        </is>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" t="inlineStr">
-        <is>
-          <t>occup_edu_2</t>
-        </is>
-      </c>
-      <c r="B24">
-        <v>6</v>
-      </c>
-      <c r="C24" t="inlineStr">
-        <is>
-          <t>university of applied sciences(Fachhochschule)</t>
-        </is>
-      </c>
-    </row>
-    <row r="25">
-      <c r="A25" t="inlineStr">
-        <is>
-          <t>occup_edu_2</t>
-        </is>
-      </c>
-      <c r="B25">
-        <v>7</v>
-      </c>
-      <c r="C25" t="inlineStr">
-        <is>
-          <t>university</t>
-        </is>
-      </c>
-    </row>
-    <row r="26">
-      <c r="A26" t="inlineStr">
-        <is>
-          <t>occup_edu_2</t>
-        </is>
-      </c>
-      <c r="B26">
-        <v>8</v>
-      </c>
-      <c r="C26" t="inlineStr">
-        <is>
-          <t>other</t>
-        </is>
-      </c>
-    </row>
-    <row r="27">
-      <c r="A27" t="inlineStr">
-        <is>
-          <t>smoker</t>
-        </is>
-      </c>
-      <c r="B27">
-        <v>1</v>
-      </c>
-      <c r="C27" t="inlineStr">
-        <is>
-          <t>Current Smoker</t>
-        </is>
-      </c>
-    </row>
-    <row r="28">
-      <c r="A28" t="inlineStr">
-        <is>
-          <t>smoker</t>
-        </is>
-      </c>
-      <c r="B28">
-        <v>2</v>
-      </c>
-      <c r="C28" t="inlineStr">
-        <is>
-          <t>Ex Smoker</t>
-        </is>
-      </c>
-    </row>
-    <row r="29">
-      <c r="A29" t="inlineStr">
-        <is>
-          <t>smoker</t>
-        </is>
-      </c>
-      <c r="B29">
-        <v>3</v>
-      </c>
-      <c r="C29" t="inlineStr">
         <is>
           <t>Never Smoker</t>
         </is>

</xml_diff>